<commit_message>
refresh the excel files
</commit_message>
<xml_diff>
--- a/git-mingling.xlsx
+++ b/git-mingling.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>编号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -174,6 +174,300 @@
   </si>
   <si>
     <t>检查当前库的状态</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rev-parse --git-dir</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rev-parse --show-toplevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示工作区的根目录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示.git目录所在的位置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rev-parse --show-prefix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>相对于工作区的相对目录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config -e --global</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑全局配置文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config -e --system</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑系统配置文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config --unset --global user.name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>删除全局文件中的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>user.name</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config --unset --global user.email</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config user.name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config user.email</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看全局文件中的用户名</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看全局文件中的用户邮件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git commit --allow-empty -m "msg"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许空白提交（无任何文件修改）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git log --pretty=fuller</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>日志全显</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git commit --amend --allow-empty --reset-author</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>--amend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>对刚刚提交进行修补</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>--allow-empty使得空表提交被允许</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>’--reset-author将</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Author</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>同步修改</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git push origin master</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>master为分支，提交到github中</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git log --state</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>查看提交日志，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>可以看到每次提交的文件变更统计</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看修改后的文件与版本库中的文件差异</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git status -s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>查看文件信息，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>简化信息量</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git checkout -- filename</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>撤销工作区尚未提交的的修改</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git ls-tree -l HEAD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>查看暂存区及</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HEAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>中的目录树</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git clean -fd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除当前工作区中没有加入版本库的文件和目录</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -232,9 +526,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -644,8 +940,171 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="C26" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>